<commit_message>
added borders to board
</commit_message>
<xml_diff>
--- a/board/bigBoard.xlsx
+++ b/board/bigBoard.xlsx
@@ -28,6 +28,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -74,7 +77,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -82,8 +85,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -106,14 +189,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="36">
     <cellStyle name="Check Cell" xfId="1" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -125,6 +239,13 @@
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -135,6 +256,13 @@
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -410,106 +538,546 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S19"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="6" style="1"/>
+    <col min="1" max="1" width="1.1640625" style="1" customWidth="1"/>
+    <col min="2" max="21" width="6" style="1"/>
+    <col min="22" max="22" width="1.1640625" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="6" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="R2" s="3"/>
-    </row>
-    <row r="3" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J4" s="3"/>
-      <c r="R4" s="3"/>
-    </row>
-    <row r="5" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="S6" s="3"/>
-    </row>
-    <row r="7" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="R8" s="3"/>
-    </row>
-    <row r="9" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="S11" s="3"/>
-    </row>
-    <row r="12" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="3"/>
-    </row>
-    <row r="14" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="S15" s="3"/>
-    </row>
-    <row r="16" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J16" s="3"/>
-      <c r="P16" s="3"/>
-    </row>
-    <row r="17" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F17" s="3"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="3"/>
-      <c r="R18" s="3"/>
-    </row>
-    <row r="19" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="P19" s="3"/>
+    <row r="1" spans="1:22" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+    </row>
+    <row r="2" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="2"/>
+    </row>
+    <row r="3" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="2"/>
+    </row>
+    <row r="4" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="2"/>
+    </row>
+    <row r="6" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="2"/>
+    </row>
+    <row r="9" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="2"/>
+    </row>
+    <row r="10" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="16"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="16"/>
+    </row>
+    <row r="12" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="19"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="19"/>
+    </row>
+    <row r="13" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="2"/>
+    </row>
+    <row r="14" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="2"/>
+    </row>
+    <row r="18" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="2"/>
+    </row>
+    <row r="19" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="2"/>
+    </row>
+    <row r="20" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="2"/>
+    </row>
+    <row r="21" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="2"/>
+    </row>
+    <row r="22" spans="1:22" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>